<commit_message>
Commiting Changes to BranchA
</commit_message>
<xml_diff>
--- a/src/test/java/com/inetBanking/testData/Guru99.xlsx
+++ b/src/test/java/com/inetBanking/testData/Guru99.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="TestCases" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="42">
   <si>
     <t>UserName</t>
   </si>
@@ -34,6 +34,114 @@
   </si>
   <si>
     <t>mngr587253</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Data required</t>
+  </si>
+  <si>
+    <t>Verify Login</t>
+  </si>
+  <si>
+    <t>Open URL</t>
+  </si>
+  <si>
+    <t>Login should successful and home page should open</t>
+  </si>
+  <si>
+    <t>UserID:mngr587250</t>
+  </si>
+  <si>
+    <t>Enter valid UserID</t>
+  </si>
+  <si>
+    <t>Password = upagunu</t>
+  </si>
+  <si>
+    <t>Enter valid Password</t>
+  </si>
+  <si>
+    <t>Clcick on login</t>
+  </si>
+  <si>
+    <t>Verify DDT testing for Login</t>
+  </si>
+  <si>
+    <t>for valid username home page should display and for invalid username we should get wrong credential popup</t>
+  </si>
+  <si>
+    <t>Enter valid UserID and invalid username</t>
+  </si>
+  <si>
+    <t>Enter valid Password and invalid username</t>
+  </si>
+  <si>
+    <t>Verify add new customer</t>
+  </si>
+  <si>
+    <t>we should get successful message</t>
+  </si>
+  <si>
+    <t>click on add customer</t>
+  </si>
+  <si>
+    <t>fill all the details</t>
+  </si>
+  <si>
+    <t>click on submit</t>
+  </si>
+  <si>
+    <t>verify edit customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edited email id should be present </t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify success message </t>
+  </si>
+  <si>
+    <t xml:space="preserve">click edit customer </t>
+  </si>
+  <si>
+    <t>enter customer id and submit</t>
+  </si>
+  <si>
+    <t>edit email id</t>
+  </si>
+  <si>
+    <t>and verify edited email id is there r not</t>
+  </si>
+  <si>
+    <t>Verify Add new Account</t>
+  </si>
+  <si>
+    <t>verify account created successful message</t>
+  </si>
+  <si>
+    <t>click add account</t>
+  </si>
+  <si>
+    <t>Enter customer id</t>
+  </si>
+  <si>
+    <t>select account type as current</t>
+  </si>
+  <si>
+    <t>enter ammount</t>
+  </si>
+  <si>
+    <t>click submit</t>
   </si>
 </sst>
 </file>
@@ -62,15 +170,21 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -78,14 +192,100 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,12 +647,346 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="31.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="45.88671875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="25.77734375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="9"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="C3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="C4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="43.2">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="C8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="C9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="E11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="6">
+        <v>3</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="C14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="C15" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="C16" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="C17" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="C18" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="C19" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="6">
+        <v>4</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="C22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="C23" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="C24" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="C25" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="C26" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="C27" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="C28" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="C29" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="C30" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="C31" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="C32" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="6">
+        <v>5</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="C35" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="C36" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="C37" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="C38" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="C39" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="C40" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="C41" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="C42" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="C43" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="C44" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="C45" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="C46" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>